<commit_message>
Update and correct Hungarian (hu-HU) translation
</commit_message>
<xml_diff>
--- a/ErgoLux/localization/Hungarian (hu-HU) translation.xlsx
+++ b/ErgoLux/localization/Hungarian (hu-HU) translation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kocsi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\ErgoLux\ErgoLux\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590AE1D-D85D-4BF0-B596-14226F60C5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5428FC4-3D1A-45AD-8230-8151F95356F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
   <sheets>
     <sheet name="hu-HU" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="565">
   <si>
     <t>Key</t>
   </si>
@@ -1282,15 +1282,9 @@
     <t>Teljesítmény (dB)</t>
   </si>
   <si>
-    <t>Szeretnél minden mezőt visszaállítani az alapértelmezett értékeikre?</t>
-  </si>
-  <si>
     <t>Beállítások visszaállítása?</t>
   </si>
   <si>
-    <t>Hiba a beállítások fájl betöltése közben. {0} Az alapértelmezett értékek lesznek alkalmazva.</t>
-  </si>
-  <si>
     <t>Hiba</t>
   </si>
   <si>
@@ -1321,9 +1315,6 @@
     <t>Hiányzik egy üres vonal.</t>
   </si>
   <si>
-    <t>Hiányzanak az oszlop fejlécek (sorozatnevek)</t>
-  </si>
-  <si>
     <t>napok, nap, napok</t>
   </si>
   <si>
@@ -1456,24 +1447,15 @@
     <t>Leállási bitek</t>
   </si>
   <si>
-    <t>Nem sikerült felállítani az adat jellegzetességeket (adat bitek, leállási bitek, és paritás)</t>
-  </si>
-  <si>
     <t>Paritás</t>
   </si>
   <si>
-    <t>Nem sikerült beállítani a Baudrátát. Hiba: {0}</t>
-  </si>
-  <si>
     <t>Baudráta hiba</t>
   </si>
   <si>
     <t>Bitek hiba</t>
   </si>
   <si>
-    <t>Az eszköz be van zárva. Kérem, menjen a Beállításokhoz hogy megnyissa az eszközt.</t>
-  </si>
-  <si>
     <t>Eszközhiba</t>
   </si>
   <si>
@@ -1486,24 +1468,12 @@
     <t>Kísérlet az FTD2XX.DLL betöltésére innen:</t>
   </si>
   <si>
-    <t>Egy váratlan hiba lépett fel az adatfájl betöltése közben. Kérem próbálja újra később, vagy vegye fel a kapcsolatot a szoftverfejlesztővel. {0}</t>
-  </si>
-  <si>
     <t>Nem sikerült megnyitni az eszközt</t>
   </si>
   <si>
-    <t>Nem sikerült megnyitni az eszközt. Hiba: {0}</t>
-  </si>
-  <si>
     <t>Hiba az eszköz megnyitása közben</t>
   </si>
   <si>
-    <t>Egy váratlan hiba lépett fel az adatok lemezre való mentése közben. Kérem próbálja újra később, vagy vegye fel a kapcsolatot a szoftverfejlesztővel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hiba a beállításfájl betöltése közben. {0} </t>
-  </si>
-  <si>
     <t>Kezdési idő</t>
   </si>
   <si>
@@ -1516,18 +1486,12 @@
     <t>Mintavételezési frekvencia</t>
   </si>
   <si>
-    <t>Ergonómiai mérő szoftvereszköz a Konica Minolta T10-A megvilágításmérőjére. Semmiféle kereskedelmi célú felhasználat nem megengedett. Vegye fel a kapcsolatot a készítővel több információért. Ha hasznosnak találja ezt a programot, kérjük fontolja meg a támogatást!</t>
-  </si>
-  <si>
     <t>Hiba a DLL betöltése közben</t>
   </si>
   <si>
     <t>Hiba az adatok betöltése közben</t>
   </si>
   <si>
-    <t>Biztos hogy ki szeretnél lépni az applikációból?</t>
-  </si>
-  <si>
     <t>Kilépés?</t>
   </si>
   <si>
@@ -1543,9 +1507,6 @@
     <t>Adatmentés</t>
   </si>
   <si>
-    <t>A Hausdorff-Besicovitch fraktáldimenzió számítása le lett állítva.</t>
-  </si>
-  <si>
     <t>Leállítás</t>
   </si>
   <si>
@@ -1576,15 +1537,9 @@
     <t>Radiáis mérőműszer</t>
   </si>
   <si>
-    <t>Nem sikerült leolvasni az adatokat ebből a fájlból. {0}</t>
-  </si>
-  <si>
     <t>Kultúranév hiba</t>
   </si>
   <si>
-    <t>A kultúra megkülönböztető stringnév érvénytelen. {0}</t>
-  </si>
-  <si>
     <t>Érvénytelen numerikus érték: {0}</t>
   </si>
   <si>
@@ -1690,12 +1645,6 @@
     <t>Adatokhoz való igazítás</t>
   </si>
   <si>
-    <t>&amp;Névjegy</t>
-  </si>
-  <si>
-    <t>Nem sikerült beállítani az áramlásszabályozást. Hiba: {0}</t>
-  </si>
-  <si>
     <t>Grafikon célkeresztjének mutatása</t>
   </si>
   <si>
@@ -1738,10 +1687,91 @@
     <t>Nincs olyan adat, ami menthető lenne.</t>
   </si>
   <si>
-    <t>Hiba történt az időtúllépések beállításában. Hiba: {0}</t>
-  </si>
-  <si>
     <t>Időtúllépési hiba</t>
+  </si>
+  <si>
+    <t>Ergonómiai mérő szoftvereszköz a Konica Minolta T10-A megvilágításmérőjére.
+Semmiféle kereskedelmi célú felhasználat nem megengedett. Vegye fel a kapcsolatot a készítővel több információért.
+Ha hasznosnak találja ezt a programot, kérjük fontolja meg a támogatást!</t>
+  </si>
+  <si>
+    <t>Hiba a beállítások fájl betöltése közben.
+{0}
+Az alapértelmezett értékek lesznek alkalmazva.</t>
+  </si>
+  <si>
+    <t>Nem sikerült felállítani az adat jellegzetességeket
+(adat bitek, leállási bitek, és paritás)
+Hiba:
+{0}</t>
+  </si>
+  <si>
+    <t>Nem sikerült beállítani a Baudrátát.
+Hiba:
+{0}</t>
+  </si>
+  <si>
+    <t>Az eszköz be van zárva. Kérem, menjen a Beállításokhoz
+hogy megnyissa az eszközt.</t>
+  </si>
+  <si>
+    <t>Nem sikerült beállítani az áramlásszabályozást.
+Hiba:
+{0}</t>
+  </si>
+  <si>
+    <t>Egy váratlan hiba lépett fel az adatfájl betöltése közben.
+Kérem próbálja újra később, vagy vegye fel a kapcsolatot a szoftverfejlesztővel.
+{0}</t>
+  </si>
+  <si>
+    <t>Nem sikerült megnyitni az eszközt.
+Hiba:
+{0}</t>
+  </si>
+  <si>
+    <t>Egy váratlan hiba lépett fel az adatok lemezre való mentése közben.
+Kérem próbálja újra később, vagy vegye fel a kapcsolatot a szoftverfejlesztővel.
+{0}</t>
+  </si>
+  <si>
+    <t>Hiba történt az időtúllépések beállításában.
+Hiba:
+{0}</t>
+  </si>
+  <si>
+    <t>Biztos hogy ki szeretnél lépni
+az applikációból?</t>
+  </si>
+  <si>
+    <t>Szeretnél minden mezőt visszaállítani
+az alapértelmezett értékeikre?</t>
+  </si>
+  <si>
+    <t>A Hausdorff-Besicovitch fraktáldimenzió
+számítása le lett állítva.</t>
+  </si>
+  <si>
+    <t>Nem sikerült leolvasni az adatokat ebből a fájlból.
+{0}</t>
+  </si>
+  <si>
+    <t>A kultúra megkülönböztető stringnév érvénytelen.
+{0}</t>
+  </si>
+  <si>
+    <t>Hiba a beállításfájl betöltése közben.
+{0}
+Az alapértelmezett értékek lesznek alkalmazva.</t>
+  </si>
+  <si>
+    <t>Hiányzanak az oszlop fejlécek (sorozatnevek).</t>
+  </si>
+  <si>
+    <t>&amp;Névjegy…</t>
+  </si>
+  <si>
+    <t>&amp;Beállítások…</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1832,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1854,7 +1884,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2152,33 +2182,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99272ECF-2233-463E-857F-E2B1C41A5F55}">
   <dimension ref="B2:AH332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C132" workbookViewId="0">
-      <selection activeCell="F136" sqref="F136"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
-    <col min="5" max="5" width="61.109375" customWidth="1"/>
-    <col min="6" max="6" width="60.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" customWidth="1"/>
-    <col min="17" max="17" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" customWidth="1"/>
+    <col min="6" max="6" width="60.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" customWidth="1"/>
     <col min="25" max="25" width="17" customWidth="1"/>
-    <col min="27" max="27" width="17.33203125" customWidth="1"/>
-    <col min="29" max="29" width="17.5546875" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" customWidth="1"/>
+    <col min="27" max="27" width="17.28515625" customWidth="1"/>
+    <col min="29" max="29" width="17.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>380</v>
       </c>
@@ -2195,7 +2223,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>381</v>
       </c>
@@ -2209,10 +2237,10 @@
         <v>363</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>381</v>
       </c>
@@ -2226,10 +2254,10 @@
         <v>365</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>381</v>
       </c>
@@ -2246,7 +2274,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>381</v>
       </c>
@@ -2263,7 +2291,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>381</v>
       </c>
@@ -2277,10 +2305,10 @@
         <v>371</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>381</v>
       </c>
@@ -2297,7 +2325,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>381</v>
       </c>
@@ -2314,7 +2342,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>381</v>
       </c>
@@ -2331,7 +2359,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>381</v>
       </c>
@@ -2345,10 +2373,10 @@
         <v>379</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>382</v>
       </c>
@@ -2365,7 +2393,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>382</v>
       </c>
@@ -2382,7 +2410,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>382</v>
       </c>
@@ -2395,11 +2423,11 @@
       <c r="E14" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>382</v>
       </c>
@@ -2416,7 +2444,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>382</v>
       </c>
@@ -2433,7 +2461,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>382</v>
       </c>
@@ -2448,7 +2476,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>382</v>
       </c>
@@ -2463,7 +2491,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>382</v>
       </c>
@@ -2478,7 +2506,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>382</v>
       </c>
@@ -2493,7 +2521,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>382</v>
       </c>
@@ -2508,7 +2536,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>382</v>
       </c>
@@ -2523,7 +2551,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>382</v>
       </c>
@@ -2535,10 +2563,10 @@
         <v>15</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>382</v>
       </c>
@@ -2553,7 +2581,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>382</v>
       </c>
@@ -2568,7 +2596,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>382</v>
       </c>
@@ -2583,7 +2611,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>382</v>
       </c>
@@ -2595,10 +2623,10 @@
         <v>169</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>382</v>
       </c>
@@ -2610,10 +2638,10 @@
         <v>171</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>382</v>
       </c>
@@ -2625,10 +2653,10 @@
         <v>173</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>382</v>
       </c>
@@ -2640,10 +2668,10 @@
         <v>175</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>382</v>
       </c>
@@ -2658,7 +2686,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>382</v>
       </c>
@@ -2670,10 +2698,10 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>382</v>
       </c>
@@ -2685,10 +2713,10 @@
         <v>26</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>382</v>
       </c>
@@ -2700,10 +2728,10 @@
         <v>28</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>382</v>
       </c>
@@ -2715,10 +2743,10 @@
         <v>30</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>382</v>
       </c>
@@ -2730,10 +2758,10 @@
         <v>31</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>382</v>
       </c>
@@ -2745,10 +2773,10 @@
         <v>34</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>382</v>
       </c>
@@ -2760,10 +2788,10 @@
         <v>36</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>382</v>
       </c>
@@ -2775,10 +2803,10 @@
         <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>382</v>
       </c>
@@ -2790,10 +2818,10 @@
         <v>58</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>382</v>
       </c>
@@ -2805,10 +2833,10 @@
         <v>40</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>382</v>
       </c>
@@ -2820,10 +2848,10 @@
         <v>42</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>382</v>
       </c>
@@ -2835,10 +2863,10 @@
         <v>176</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>382</v>
       </c>
@@ -2853,7 +2881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>382</v>
       </c>
@@ -2865,10 +2893,10 @@
         <v>44</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>382</v>
       </c>
@@ -2883,7 +2911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>382</v>
       </c>
@@ -2895,10 +2923,10 @@
         <v>177</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>382</v>
       </c>
@@ -2913,7 +2941,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>382</v>
       </c>
@@ -2925,10 +2953,10 @@
         <v>179</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>382</v>
       </c>
@@ -2940,10 +2968,10 @@
         <v>44</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>382</v>
       </c>
@@ -2955,10 +2983,10 @@
         <v>180</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>382</v>
       </c>
@@ -2970,10 +2998,10 @@
         <v>60</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>382</v>
       </c>
@@ -2985,10 +3013,10 @@
         <v>62</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>382</v>
       </c>
@@ -3000,10 +3028,10 @@
         <v>384</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>382</v>
       </c>
@@ -3015,10 +3043,10 @@
         <v>385</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>382</v>
       </c>
@@ -3030,10 +3058,10 @@
         <v>386</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>382</v>
       </c>
@@ -3045,10 +3073,10 @@
         <v>387</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>382</v>
       </c>
@@ -3060,10 +3088,10 @@
         <v>67</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>382</v>
       </c>
@@ -3075,10 +3103,10 @@
         <v>388</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>382</v>
       </c>
@@ -3093,7 +3121,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>382</v>
       </c>
@@ -3105,10 +3133,10 @@
         <v>69</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>382</v>
       </c>
@@ -3123,7 +3151,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>382</v>
       </c>
@@ -3135,10 +3163,10 @@
         <v>71</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>382</v>
       </c>
@@ -3150,10 +3178,10 @@
         <v>73</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>382</v>
       </c>
@@ -3165,10 +3193,10 @@
         <v>75</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>382</v>
       </c>
@@ -3183,7 +3211,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>382</v>
       </c>
@@ -3195,10 +3223,10 @@
         <v>184</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>382</v>
       </c>
@@ -3210,10 +3238,10 @@
         <v>186</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>382</v>
       </c>
@@ -3225,10 +3253,10 @@
         <v>188</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>382</v>
       </c>
@@ -3240,10 +3268,10 @@
         <v>190</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>382</v>
       </c>
@@ -3255,10 +3283,10 @@
         <v>192</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>382</v>
       </c>
@@ -3270,10 +3298,10 @@
         <v>194</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>382</v>
       </c>
@@ -3285,10 +3313,10 @@
         <v>196</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>382</v>
       </c>
@@ -3300,10 +3328,10 @@
         <v>79</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>382</v>
       </c>
@@ -3315,10 +3343,10 @@
         <v>81</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>382</v>
       </c>
@@ -3330,10 +3358,10 @@
         <v>171</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>382</v>
       </c>
@@ -3345,10 +3373,10 @@
         <v>199</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>382</v>
       </c>
@@ -3360,10 +3388,10 @@
         <v>201</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>382</v>
       </c>
@@ -3375,10 +3403,10 @@
         <v>83</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>382</v>
       </c>
@@ -3390,10 +3418,10 @@
         <v>203</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>382</v>
       </c>
@@ -3405,10 +3433,10 @@
         <v>85</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>382</v>
       </c>
@@ -3420,10 +3448,10 @@
         <v>205</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>382</v>
       </c>
@@ -3435,10 +3463,10 @@
         <v>206</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>382</v>
       </c>
@@ -3450,10 +3478,10 @@
         <v>208</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>382</v>
       </c>
@@ -3465,10 +3493,10 @@
         <v>113</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>382</v>
       </c>
@@ -3480,10 +3508,10 @@
         <v>211</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>382</v>
       </c>
@@ -3495,10 +3523,10 @@
         <v>213</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>382</v>
       </c>
@@ -3510,10 +3538,10 @@
         <v>215</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>382</v>
       </c>
@@ -3525,10 +3553,10 @@
         <v>217</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>382</v>
       </c>
@@ -3540,10 +3568,10 @@
         <v>58</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>382</v>
       </c>
@@ -3555,10 +3583,10 @@
         <v>88</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>382</v>
       </c>
@@ -3570,10 +3598,10 @@
         <v>90</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>382</v>
       </c>
@@ -3585,10 +3613,10 @@
         <v>220</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>382</v>
       </c>
@@ -3600,10 +3628,10 @@
         <v>92</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>382</v>
       </c>
@@ -3615,10 +3643,10 @@
         <v>222</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>382</v>
       </c>
@@ -3630,10 +3658,10 @@
         <v>224</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>382</v>
       </c>
@@ -3645,10 +3673,10 @@
         <v>226</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>382</v>
       </c>
@@ -3660,10 +3688,10 @@
         <v>228</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>382</v>
       </c>
@@ -3675,10 +3703,10 @@
         <v>230</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>382</v>
       </c>
@@ -3690,10 +3718,10 @@
         <v>232</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>382</v>
       </c>
@@ -3705,10 +3733,10 @@
         <v>234</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>382</v>
       </c>
@@ -3720,10 +3748,10 @@
         <v>236</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>382</v>
       </c>
@@ -3735,10 +3763,10 @@
         <v>238</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>382</v>
       </c>
@@ -3750,10 +3778,10 @@
         <v>240</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>382</v>
       </c>
@@ -3765,10 +3793,10 @@
         <v>242</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
         <v>382</v>
       </c>
@@ -3780,10 +3808,10 @@
         <v>244</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
         <v>382</v>
       </c>
@@ -3795,10 +3823,10 @@
         <v>246</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
         <v>382</v>
       </c>
@@ -3810,10 +3838,10 @@
         <v>248</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
         <v>382</v>
       </c>
@@ -3825,10 +3853,10 @@
         <v>250</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
         <v>382</v>
       </c>
@@ -3840,10 +3868,10 @@
         <v>252</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
         <v>382</v>
       </c>
@@ -3855,10 +3883,10 @@
         <v>254</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>382</v>
       </c>
@@ -3870,10 +3898,10 @@
         <v>256</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>382</v>
       </c>
@@ -3885,10 +3913,10 @@
         <v>258</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>382</v>
       </c>
@@ -3900,10 +3928,10 @@
         <v>260</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
         <v>382</v>
       </c>
@@ -3915,10 +3943,10 @@
         <v>262</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
         <v>382</v>
       </c>
@@ -3930,10 +3958,10 @@
         <v>264</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>382</v>
       </c>
@@ -3945,10 +3973,10 @@
         <v>266</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
         <v>382</v>
       </c>
@@ -3960,10 +3988,10 @@
         <v>268</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
         <v>382</v>
       </c>
@@ -3975,10 +4003,10 @@
         <v>270</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
         <v>382</v>
       </c>
@@ -3990,10 +4018,10 @@
         <v>272</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>382</v>
       </c>
@@ -4005,10 +4033,10 @@
         <v>274</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>382</v>
       </c>
@@ -4020,10 +4048,10 @@
         <v>276</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
         <v>382</v>
       </c>
@@ -4035,10 +4063,10 @@
         <v>278</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
         <v>382</v>
       </c>
@@ -4050,10 +4078,10 @@
         <v>94</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
         <v>382</v>
       </c>
@@ -4065,10 +4093,10 @@
         <v>96</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
         <v>382</v>
       </c>
@@ -4080,10 +4108,10 @@
         <v>280</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
         <v>382</v>
       </c>
@@ -4095,10 +4123,10 @@
         <v>30</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
         <v>382</v>
       </c>
@@ -4110,10 +4138,10 @@
         <v>283</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>382</v>
       </c>
@@ -4125,10 +4153,10 @@
         <v>285</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>382</v>
       </c>
@@ -4140,10 +4168,10 @@
         <v>286</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>382</v>
       </c>
@@ -4155,10 +4183,10 @@
         <v>99</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
         <v>382</v>
       </c>
@@ -4170,10 +4198,10 @@
         <v>28</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
         <v>382</v>
       </c>
@@ -4185,10 +4213,10 @@
         <v>30</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
         <v>382</v>
       </c>
@@ -4200,10 +4228,10 @@
         <v>290</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>382</v>
       </c>
@@ -4215,10 +4243,10 @@
         <v>292</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
         <v>382</v>
       </c>
@@ -4230,10 +4258,10 @@
         <v>101</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>382</v>
       </c>
@@ -4245,10 +4273,10 @@
         <v>103</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
         <v>382</v>
       </c>
@@ -4260,10 +4288,10 @@
         <v>105</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
         <v>382</v>
       </c>
@@ -4275,10 +4303,10 @@
         <v>107</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="140" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
         <v>382</v>
       </c>
@@ -4290,10 +4318,10 @@
         <v>24</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>382</v>
       </c>
@@ -4305,10 +4333,10 @@
         <v>295</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
         <v>382</v>
       </c>
@@ -4320,10 +4348,10 @@
         <v>108</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
         <v>382</v>
       </c>
@@ -4335,10 +4363,10 @@
         <v>298</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="144" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>382</v>
       </c>
@@ -4350,10 +4378,10 @@
         <v>109</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>382</v>
       </c>
@@ -4365,10 +4393,10 @@
         <v>301</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="146" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>382</v>
       </c>
@@ -4380,10 +4408,10 @@
         <v>322</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
         <v>382</v>
       </c>
@@ -4395,10 +4423,10 @@
         <v>302</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
         <v>382</v>
       </c>
@@ -4410,10 +4438,10 @@
         <v>304</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
         <v>382</v>
       </c>
@@ -4425,10 +4453,10 @@
         <v>112</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
         <v>382</v>
       </c>
@@ -4443,7 +4471,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
         <v>382</v>
       </c>
@@ -4455,10 +4483,10 @@
         <v>309</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
         <v>382</v>
       </c>
@@ -4470,10 +4498,10 @@
         <v>311</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
         <v>382</v>
       </c>
@@ -4485,10 +4513,10 @@
         <v>112</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="s">
         <v>382</v>
       </c>
@@ -4500,10 +4528,10 @@
         <v>314</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
         <v>382</v>
       </c>
@@ -4515,10 +4543,10 @@
         <v>180</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
         <v>382</v>
       </c>
@@ -4530,10 +4558,10 @@
         <v>112</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
         <v>382</v>
       </c>
@@ -4548,7 +4576,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
         <v>382</v>
       </c>
@@ -4560,10 +4588,10 @@
         <v>115</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
         <v>382</v>
       </c>
@@ -4575,10 +4603,10 @@
         <v>117</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
         <v>382</v>
       </c>
@@ -4593,7 +4621,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
         <v>382</v>
       </c>
@@ -4605,10 +4633,10 @@
         <v>321</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
         <v>382</v>
       </c>
@@ -4620,10 +4648,10 @@
         <v>71</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="163" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="163" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
         <v>382</v>
       </c>
@@ -4635,10 +4663,10 @@
         <v>120</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="164" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="164" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
         <v>382</v>
       </c>
@@ -4650,10 +4678,10 @@
         <v>122</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
         <v>382</v>
       </c>
@@ -4665,10 +4693,10 @@
         <v>124</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
         <v>382</v>
       </c>
@@ -4680,10 +4708,10 @@
         <v>126</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
         <v>382</v>
       </c>
@@ -4695,10 +4723,10 @@
         <v>128</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
         <v>382</v>
       </c>
@@ -4710,10 +4738,10 @@
         <v>96</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="169" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
         <v>382</v>
       </c>
@@ -4725,10 +4753,10 @@
         <v>322</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>382</v>
       </c>
@@ -4740,10 +4768,10 @@
         <v>323</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
         <v>382</v>
       </c>
@@ -4755,10 +4783,10 @@
         <v>325</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>382</v>
       </c>
@@ -4770,10 +4798,10 @@
         <v>327</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
         <v>382</v>
       </c>
@@ -4785,10 +4813,10 @@
         <v>192</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B174" s="1" t="s">
         <v>382</v>
       </c>
@@ -4800,10 +4828,10 @@
         <v>330</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="s">
         <v>382</v>
       </c>
@@ -4815,10 +4843,10 @@
         <v>133</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="s">
         <v>382</v>
       </c>
@@ -4830,10 +4858,10 @@
         <v>171</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="177" spans="2:34" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="177" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
         <v>382</v>
       </c>
@@ -4845,10 +4873,10 @@
         <v>333</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="178" spans="2:34" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="178" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B178" s="1" t="s">
         <v>382</v>
       </c>
@@ -4860,10 +4888,10 @@
         <v>327</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="179" spans="2:34" x14ac:dyDescent="0.3">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="179" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B179" s="1" t="s">
         <v>382</v>
       </c>
@@ -4875,10 +4903,10 @@
         <v>336</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="180" spans="2:34" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="180" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
         <v>382</v>
       </c>
@@ -4890,10 +4918,10 @@
         <v>338</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="181" spans="2:34" x14ac:dyDescent="0.3">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="181" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
         <v>382</v>
       </c>
@@ -4905,10 +4933,10 @@
         <v>340</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="182" spans="2:34" x14ac:dyDescent="0.3">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="182" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
         <v>382</v>
       </c>
@@ -4920,12 +4948,12 @@
         <v>173</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="N182" s="2"/>
       <c r="P182" s="2"/>
     </row>
-    <row r="183" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="s">
         <v>382</v>
       </c>
@@ -4937,10 +4965,10 @@
         <v>175</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="184" spans="2:34" x14ac:dyDescent="0.3">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="184" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="s">
         <v>382</v>
       </c>
@@ -4952,7 +4980,7 @@
         <v>344</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="H184" s="2"/>
       <c r="N184" s="2"/>
@@ -4964,7 +4992,7 @@
       <c r="AD184" s="2"/>
       <c r="AF184" s="2"/>
     </row>
-    <row r="185" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
         <v>382</v>
       </c>
@@ -4976,10 +5004,10 @@
         <v>344</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="186" spans="2:34" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="186" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B186" s="1" t="s">
         <v>382</v>
       </c>
@@ -4991,7 +5019,7 @@
         <v>347</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="H186" s="2"/>
       <c r="J186" s="2"/>
@@ -5008,7 +5036,7 @@
       <c r="AF186" s="2"/>
       <c r="AH186" s="2"/>
     </row>
-    <row r="187" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B187" s="1" t="s">
         <v>382</v>
       </c>
@@ -5020,10 +5048,10 @@
         <v>135</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="188" spans="2:34" x14ac:dyDescent="0.3">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="188" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B188" s="1" t="s">
         <v>382</v>
       </c>
@@ -5035,10 +5063,10 @@
         <v>349</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="189" spans="2:34" x14ac:dyDescent="0.3">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="189" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
         <v>382</v>
       </c>
@@ -5050,10 +5078,10 @@
         <v>137</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="190" spans="2:34" x14ac:dyDescent="0.3">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="190" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B190" s="1" t="s">
         <v>382</v>
       </c>
@@ -5065,10 +5093,10 @@
         <v>351</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="191" spans="2:34" x14ac:dyDescent="0.3">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="191" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B191" s="1" t="s">
         <v>382</v>
       </c>
@@ -5080,10 +5108,10 @@
         <v>353</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="192" spans="2:34" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="192" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B192" s="1" t="s">
         <v>382</v>
       </c>
@@ -5095,10 +5123,10 @@
         <v>139</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="193" spans="2:28" x14ac:dyDescent="0.3">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="193" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B193" s="1" t="s">
         <v>382</v>
       </c>
@@ -5110,10 +5138,10 @@
         <v>141</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="194" spans="2:28" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="194" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B194" s="1" t="s">
         <v>382</v>
       </c>
@@ -5125,10 +5153,10 @@
         <v>355</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="195" spans="2:28" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="195" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B195" s="1" t="s">
         <v>382</v>
       </c>
@@ -5140,10 +5168,10 @@
         <v>73</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="196" spans="2:28" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="196" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B196" s="1" t="s">
         <v>382</v>
       </c>
@@ -5155,10 +5183,10 @@
         <v>144</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="197" spans="2:28" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="197" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
         <v>382</v>
       </c>
@@ -5170,10 +5198,10 @@
         <v>357</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="198" spans="2:28" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="198" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
         <v>382</v>
       </c>
@@ -5185,10 +5213,10 @@
         <v>359</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="199" spans="2:28" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="199" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B199" s="1" t="s">
         <v>382</v>
       </c>
@@ -5200,10 +5228,10 @@
         <v>146</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="200" spans="2:28" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="200" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B200" s="1" t="s">
         <v>382</v>
       </c>
@@ -5215,7 +5243,7 @@
         <v>148</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="L200" s="2"/>
       <c r="N200" s="2"/>
@@ -5224,7 +5252,7 @@
       <c r="X200" s="2"/>
       <c r="Z200" s="2"/>
     </row>
-    <row r="201" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
         <v>382</v>
       </c>
@@ -5236,10 +5264,10 @@
         <v>361</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="202" spans="2:28" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="202" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="s">
         <v>382</v>
       </c>
@@ -5251,7 +5279,7 @@
         <v>150</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="H202" s="2"/>
       <c r="J202" s="2"/>
@@ -5265,7 +5293,7 @@
       <c r="Z202" s="2"/>
       <c r="AB202" s="2"/>
     </row>
-    <row r="203" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B203" s="1" t="s">
         <v>382</v>
       </c>
@@ -5277,10 +5305,10 @@
         <v>152</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="229" spans="6:34" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="229" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F229" s="2"/>
       <c r="H229" s="2"/>
       <c r="J229" s="2"/>
@@ -5296,7 +5324,7 @@
       <c r="AF229" s="2"/>
       <c r="AH229" s="2"/>
     </row>
-    <row r="231" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="231" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F231" s="2"/>
       <c r="H231" s="2"/>
       <c r="J231" s="2"/>
@@ -5313,7 +5341,7 @@
       <c r="AF231" s="2"/>
       <c r="AH231" s="2"/>
     </row>
-    <row r="233" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="233" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F233" s="2"/>
       <c r="H233" s="2"/>
       <c r="J233" s="2"/>
@@ -5330,7 +5358,7 @@
       <c r="AF233" s="2"/>
       <c r="AH233" s="2"/>
     </row>
-    <row r="235" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="235" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F235" s="2"/>
       <c r="H235" s="2"/>
       <c r="J235" s="2"/>
@@ -5342,7 +5370,7 @@
       <c r="AD235" s="2"/>
       <c r="AF235" s="2"/>
     </row>
-    <row r="237" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="237" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F237" s="2"/>
       <c r="H237" s="2"/>
       <c r="J237" s="2"/>
@@ -5358,7 +5386,7 @@
       <c r="AF237" s="2"/>
       <c r="AH237" s="2"/>
     </row>
-    <row r="243" spans="6:32" x14ac:dyDescent="0.3">
+    <row r="243" spans="6:32" x14ac:dyDescent="0.25">
       <c r="F243" s="2"/>
       <c r="H243" s="2"/>
       <c r="J243" s="2"/>
@@ -5372,7 +5400,7 @@
       <c r="AD243" s="2"/>
       <c r="AF243" s="2"/>
     </row>
-    <row r="273" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="273" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F273" s="2"/>
       <c r="H273" s="2"/>
       <c r="J273" s="2"/>
@@ -5389,7 +5417,7 @@
       <c r="AF273" s="2"/>
       <c r="AH273" s="2"/>
     </row>
-    <row r="274" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="274" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F274" s="2"/>
       <c r="H274" s="2"/>
       <c r="J274" s="2"/>
@@ -5406,35 +5434,35 @@
       <c r="AF274" s="2"/>
       <c r="AH274" s="2"/>
     </row>
-    <row r="280" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="280" spans="6:34" x14ac:dyDescent="0.25">
       <c r="N280" s="2"/>
       <c r="P280" s="2"/>
       <c r="V280" s="2"/>
       <c r="X280" s="2"/>
       <c r="Z280" s="2"/>
     </row>
-    <row r="281" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="281" spans="6:34" x14ac:dyDescent="0.25">
       <c r="N281" s="2"/>
       <c r="P281" s="2"/>
       <c r="V281" s="2"/>
       <c r="X281" s="2"/>
       <c r="Z281" s="2"/>
     </row>
-    <row r="284" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="284" spans="6:34" x14ac:dyDescent="0.25">
       <c r="N284" s="2"/>
       <c r="P284" s="2"/>
       <c r="V284" s="2"/>
       <c r="X284" s="2"/>
       <c r="Z284" s="2"/>
     </row>
-    <row r="288" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="288" spans="6:34" x14ac:dyDescent="0.25">
       <c r="N288" s="2"/>
       <c r="P288" s="2"/>
       <c r="V288" s="2"/>
       <c r="X288" s="2"/>
       <c r="Z288" s="2"/>
     </row>
-    <row r="292" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="292" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F292" s="2"/>
       <c r="H292" s="2"/>
       <c r="J292" s="2"/>
@@ -5448,7 +5476,7 @@
       <c r="Z292" s="2"/>
       <c r="AB292" s="2"/>
     </row>
-    <row r="296" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="296" spans="6:28" x14ac:dyDescent="0.25">
       <c r="L296" s="2"/>
       <c r="N296" s="2"/>
       <c r="P296" s="2"/>
@@ -5456,7 +5484,7 @@
       <c r="X296" s="2"/>
       <c r="Z296" s="2"/>
     </row>
-    <row r="298" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="298" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F298" s="2"/>
       <c r="H298" s="2"/>
       <c r="J298" s="2"/>
@@ -5470,7 +5498,7 @@
       <c r="Z298" s="2"/>
       <c r="AB298" s="2"/>
     </row>
-    <row r="300" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="300" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F300" s="2"/>
       <c r="H300" s="2"/>
       <c r="J300" s="2"/>
@@ -5484,7 +5512,7 @@
       <c r="Z300" s="2"/>
       <c r="AB300" s="2"/>
     </row>
-    <row r="302" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="302" spans="6:28" x14ac:dyDescent="0.25">
       <c r="L302" s="2"/>
       <c r="N302" s="2"/>
       <c r="P302" s="2"/>
@@ -5492,7 +5520,7 @@
       <c r="X302" s="2"/>
       <c r="Z302" s="2"/>
     </row>
-    <row r="304" spans="6:28" x14ac:dyDescent="0.3">
+    <row r="304" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F304" s="2"/>
       <c r="H304" s="2"/>
       <c r="L304" s="2"/>
@@ -5502,7 +5530,7 @@
       <c r="Z304" s="2"/>
       <c r="AB304" s="2"/>
     </row>
-    <row r="308" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="308" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F308" s="2"/>
       <c r="H308" s="2"/>
       <c r="L308" s="2"/>
@@ -5513,10 +5541,10 @@
       <c r="Z308" s="2"/>
       <c r="AB308" s="2"/>
     </row>
-    <row r="310" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="310" spans="6:34" x14ac:dyDescent="0.25">
       <c r="P310" s="2"/>
     </row>
-    <row r="312" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="312" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F312" s="2"/>
       <c r="H312" s="2"/>
       <c r="J312" s="2"/>
@@ -5529,31 +5557,31 @@
       <c r="Z312" s="2"/>
       <c r="AB312" s="2"/>
     </row>
-    <row r="320" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="320" spans="6:34" x14ac:dyDescent="0.25">
       <c r="L320" s="2"/>
       <c r="N320" s="2"/>
       <c r="P320" s="2"/>
       <c r="AH320" s="2"/>
     </row>
-    <row r="323" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="323" spans="6:34" x14ac:dyDescent="0.25">
       <c r="L323" s="2"/>
       <c r="N323" s="2"/>
       <c r="P323" s="2"/>
       <c r="AH323" s="2"/>
     </row>
-    <row r="324" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="324" spans="6:34" x14ac:dyDescent="0.25">
       <c r="L324" s="2"/>
       <c r="N324" s="2"/>
       <c r="P324" s="2"/>
       <c r="AH324" s="2"/>
     </row>
-    <row r="326" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="326" spans="6:34" x14ac:dyDescent="0.25">
       <c r="L326" s="2"/>
       <c r="N326" s="2"/>
       <c r="P326" s="2"/>
       <c r="AH326" s="2"/>
     </row>
-    <row r="331" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="331" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F331" s="2"/>
       <c r="H331" s="2"/>
       <c r="J331" s="2"/>
@@ -5567,7 +5595,7 @@
       <c r="Z331" s="2"/>
       <c r="AB331" s="2"/>
     </row>
-    <row r="332" spans="6:34" x14ac:dyDescent="0.3">
+    <row r="332" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F332" s="2"/>
       <c r="H332" s="2"/>
       <c r="J332" s="2"/>

</xml_diff>